<commit_message>
Added parts to all fake users
</commit_message>
<xml_diff>
--- a/spec/fixtures/FakeUsers.xlsx
+++ b/spec/fixtures/FakeUsers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/models/mock-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="698">
   <si>
     <t>Spot</t>
   </si>
@@ -2557,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171:D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3830,7 +3830,9 @@
       <c r="C44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="6"/>
+      <c r="D44" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E44" s="4" t="s">
         <v>515</v>
       </c>
@@ -3857,7 +3859,9 @@
       <c r="C45" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="6"/>
+      <c r="D45" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E45" s="4" t="s">
         <v>516</v>
       </c>
@@ -3884,7 +3888,9 @@
       <c r="C46" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="6"/>
+      <c r="D46" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E46" s="4" t="s">
         <v>517</v>
       </c>
@@ -3911,7 +3917,9 @@
       <c r="C47" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="6"/>
+      <c r="D47" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E47" s="4" t="s">
         <v>518</v>
       </c>
@@ -3938,7 +3946,9 @@
       <c r="C48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="6"/>
+      <c r="D48" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E48" s="4" t="s">
         <v>519</v>
       </c>
@@ -3965,7 +3975,9 @@
       <c r="C49" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="6"/>
+      <c r="D49" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E49" s="4" t="s">
         <v>520</v>
       </c>
@@ -3992,7 +4004,9 @@
       <c r="C50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E50" s="4" t="s">
         <v>521</v>
       </c>
@@ -4019,7 +4033,9 @@
       <c r="C51" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="6"/>
+      <c r="D51" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E51" s="4" t="s">
         <v>522</v>
       </c>
@@ -4046,7 +4062,9 @@
       <c r="C52" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E52" s="4" t="s">
         <v>523</v>
       </c>
@@ -4073,7 +4091,9 @@
       <c r="C53" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="6"/>
+      <c r="D53" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E53" s="4" t="s">
         <v>524</v>
       </c>
@@ -4100,7 +4120,9 @@
       <c r="C54" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="6"/>
+      <c r="D54" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E54" s="4" t="s">
         <v>525</v>
       </c>
@@ -4127,7 +4149,9 @@
       <c r="C55" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="6"/>
+      <c r="D55" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E55" s="4" t="s">
         <v>526</v>
       </c>
@@ -4154,7 +4178,9 @@
       <c r="C56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="6"/>
+      <c r="D56" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E56" s="4" t="s">
         <v>527</v>
       </c>
@@ -4181,7 +4207,9 @@
       <c r="C57" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="E57" s="4" t="s">
         <v>528</v>
       </c>
@@ -4615,7 +4643,9 @@
       <c r="C72" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D72" s="6"/>
+      <c r="D72" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E72" s="4" t="s">
         <v>543</v>
       </c>
@@ -4642,7 +4672,9 @@
       <c r="C73" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D73" s="6"/>
+      <c r="D73" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E73" s="4" t="s">
         <v>544</v>
       </c>
@@ -4669,7 +4701,9 @@
       <c r="C74" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="6"/>
+      <c r="D74" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E74" s="4" t="s">
         <v>545</v>
       </c>
@@ -4696,7 +4730,9 @@
       <c r="C75" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D75" s="6"/>
+      <c r="D75" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E75" s="4" t="s">
         <v>546</v>
       </c>
@@ -4723,7 +4759,9 @@
       <c r="C76" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="6"/>
+      <c r="D76" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E76" s="4" t="s">
         <v>547</v>
       </c>
@@ -4750,7 +4788,9 @@
       <c r="C77" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D77" s="6"/>
+      <c r="D77" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E77" s="4" t="s">
         <v>548</v>
       </c>
@@ -4777,7 +4817,9 @@
       <c r="C78" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D78" s="6"/>
+      <c r="D78" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E78" s="4" t="s">
         <v>549</v>
       </c>
@@ -4804,7 +4846,9 @@
       <c r="C79" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E79" s="4" t="s">
         <v>550</v>
       </c>
@@ -4831,7 +4875,9 @@
       <c r="C80" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E80" s="4" t="s">
         <v>469</v>
       </c>
@@ -4858,7 +4904,9 @@
       <c r="C81" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D81" s="6"/>
+      <c r="D81" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E81" s="4" t="s">
         <v>551</v>
       </c>
@@ -4886,7 +4934,9 @@
       <c r="C82" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D82" s="6"/>
+      <c r="D82" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E82" s="4" t="s">
         <v>552</v>
       </c>
@@ -4914,7 +4964,9 @@
       <c r="C83" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D83" s="6"/>
+      <c r="D83" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E83" s="4" t="s">
         <v>553</v>
       </c>
@@ -4941,7 +4993,9 @@
       <c r="C84" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D84" s="6"/>
+      <c r="D84" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E84" s="4" t="s">
         <v>554</v>
       </c>
@@ -4968,7 +5022,9 @@
       <c r="C85" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D85" s="8"/>
+      <c r="D85" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E85" s="4" t="s">
         <v>555</v>
       </c>
@@ -4995,7 +5051,9 @@
       <c r="C86" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D86" s="6"/>
+      <c r="D86" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E86" s="4" t="s">
         <v>556</v>
       </c>
@@ -5022,7 +5080,9 @@
       <c r="C87" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D87" s="6"/>
+      <c r="D87" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E87" s="4" t="s">
         <v>557</v>
       </c>
@@ -5049,7 +5109,9 @@
       <c r="C88" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D88" s="6"/>
+      <c r="D88" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E88" s="4" t="s">
         <v>558</v>
       </c>
@@ -5077,7 +5139,9 @@
       <c r="C89" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D89" s="6"/>
+      <c r="D89" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E89" s="4" t="s">
         <v>559</v>
       </c>
@@ -5104,7 +5168,9 @@
       <c r="C90" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E90" s="4" t="s">
         <v>560</v>
       </c>
@@ -5131,7 +5197,9 @@
       <c r="C91" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D91" s="6"/>
+      <c r="D91" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E91" s="4" t="s">
         <v>561</v>
       </c>
@@ -5158,7 +5226,9 @@
       <c r="C92" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D92" s="6"/>
+      <c r="D92" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E92" s="4" t="s">
         <v>562</v>
       </c>
@@ -5185,7 +5255,9 @@
       <c r="C93" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D93" s="6"/>
+      <c r="D93" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E93" s="4" t="s">
         <v>563</v>
       </c>
@@ -5212,7 +5284,9 @@
       <c r="C94" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D94" s="6"/>
+      <c r="D94" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E94" s="4" t="s">
         <v>564</v>
       </c>
@@ -5239,7 +5313,9 @@
       <c r="C95" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D95" s="6"/>
+      <c r="D95" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E95" s="4" t="s">
         <v>565</v>
       </c>
@@ -5266,7 +5342,9 @@
       <c r="C96" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D96" s="6"/>
+      <c r="D96" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E96" s="4" t="s">
         <v>566</v>
       </c>
@@ -5293,7 +5371,9 @@
       <c r="C97" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D97" s="6"/>
+      <c r="D97" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E97" s="4" t="s">
         <v>567</v>
       </c>
@@ -5320,7 +5400,9 @@
       <c r="C98" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D98" s="6"/>
+      <c r="D98" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E98" s="4" t="s">
         <v>568</v>
       </c>
@@ -5347,7 +5429,9 @@
       <c r="C99" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D99" s="8"/>
+      <c r="D99" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E99" s="4" t="s">
         <v>569</v>
       </c>
@@ -5374,7 +5458,9 @@
       <c r="C100" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D100" s="6"/>
+      <c r="D100" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E100" s="4" t="s">
         <v>570</v>
       </c>
@@ -5401,7 +5487,9 @@
       <c r="C101" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D101" s="6"/>
+      <c r="D101" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E101" s="4" t="s">
         <v>571</v>
       </c>
@@ -5428,7 +5516,9 @@
       <c r="C102" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D102" s="6"/>
+      <c r="D102" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E102" s="4" t="s">
         <v>572</v>
       </c>
@@ -5455,7 +5545,9 @@
       <c r="C103" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D103" s="6"/>
+      <c r="D103" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E103" s="4" t="s">
         <v>573</v>
       </c>
@@ -5482,7 +5574,9 @@
       <c r="C104" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D104" s="6"/>
+      <c r="D104" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E104" s="4" t="s">
         <v>574</v>
       </c>
@@ -5509,7 +5603,9 @@
       <c r="C105" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D105" s="6"/>
+      <c r="D105" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E105" s="4" t="s">
         <v>575</v>
       </c>
@@ -5536,7 +5632,9 @@
       <c r="C106" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D106" s="6"/>
+      <c r="D106" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E106" s="4" t="s">
         <v>576</v>
       </c>
@@ -5563,7 +5661,9 @@
       <c r="C107" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D107" s="6"/>
+      <c r="D107" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E107" s="4" t="s">
         <v>577</v>
       </c>
@@ -5590,7 +5690,9 @@
       <c r="C108" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D108" s="6"/>
+      <c r="D108" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E108" s="4" t="s">
         <v>578</v>
       </c>
@@ -5617,7 +5719,9 @@
       <c r="C109" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D109" s="6"/>
+      <c r="D109" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E109" s="4" t="s">
         <v>579</v>
       </c>
@@ -5644,7 +5748,9 @@
       <c r="C110" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D110" s="6"/>
+      <c r="D110" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E110" s="4" t="s">
         <v>580</v>
       </c>
@@ -5672,7 +5778,9 @@
       <c r="C111" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D111" s="6"/>
+      <c r="D111" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E111" s="4" t="s">
         <v>581</v>
       </c>
@@ -5699,7 +5807,9 @@
       <c r="C112" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D112" s="6"/>
+      <c r="D112" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E112" s="4" t="s">
         <v>582</v>
       </c>
@@ -5726,7 +5836,9 @@
       <c r="C113" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D113" s="6"/>
+      <c r="D113" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E113" s="4" t="s">
         <v>583</v>
       </c>
@@ -5753,7 +5865,9 @@
       <c r="C114" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D114" s="8"/>
+      <c r="D114" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E114" s="4" t="s">
         <v>584</v>
       </c>
@@ -5780,7 +5894,9 @@
       <c r="C115" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D115" s="6"/>
+      <c r="D115" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E115" s="4" t="s">
         <v>585</v>
       </c>
@@ -5807,7 +5923,9 @@
       <c r="C116" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D116" s="6"/>
+      <c r="D116" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E116" s="4" t="s">
         <v>586</v>
       </c>
@@ -5834,7 +5952,9 @@
       <c r="C117" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D117" s="6"/>
+      <c r="D117" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E117" s="4" t="s">
         <v>587</v>
       </c>
@@ -5862,7 +5982,9 @@
       <c r="C118" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D118" s="6"/>
+      <c r="D118" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E118" s="4" t="s">
         <v>588</v>
       </c>
@@ -5889,7 +6011,9 @@
       <c r="C119" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D119" s="6"/>
+      <c r="D119" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E119" s="4" t="s">
         <v>589</v>
       </c>
@@ -5916,7 +6040,9 @@
       <c r="C120" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D120" s="6"/>
+      <c r="D120" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E120" s="4" t="s">
         <v>470</v>
       </c>
@@ -5943,7 +6069,9 @@
       <c r="C121" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D121" s="6"/>
+      <c r="D121" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E121" s="4" t="s">
         <v>590</v>
       </c>
@@ -5970,7 +6098,9 @@
       <c r="C122" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D122" s="6"/>
+      <c r="D122" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E122" s="4" t="s">
         <v>591</v>
       </c>
@@ -5997,7 +6127,9 @@
       <c r="C123" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D123" s="6"/>
+      <c r="D123" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E123" s="4" t="s">
         <v>592</v>
       </c>
@@ -6024,7 +6156,9 @@
       <c r="C124" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D124" s="6"/>
+      <c r="D124" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E124" s="4" t="s">
         <v>593</v>
       </c>
@@ -6051,7 +6185,9 @@
       <c r="C125" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D125" s="6"/>
+      <c r="D125" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E125" s="4" t="s">
         <v>594</v>
       </c>
@@ -6078,7 +6214,9 @@
       <c r="C126" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D126" s="6"/>
+      <c r="D126" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E126" s="4" t="s">
         <v>595</v>
       </c>
@@ -6105,7 +6243,9 @@
       <c r="C127" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="6"/>
+      <c r="D127" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E127" s="4" t="s">
         <v>596</v>
       </c>
@@ -6132,7 +6272,9 @@
       <c r="C128" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D128" s="8"/>
+      <c r="D128" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E128" s="4" t="s">
         <v>597</v>
       </c>
@@ -6159,7 +6301,9 @@
       <c r="C129" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D129" s="6"/>
+      <c r="D129" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E129" s="4" t="s">
         <v>598</v>
       </c>
@@ -6186,7 +6330,9 @@
       <c r="C130" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D130" s="6"/>
+      <c r="D130" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E130" s="4" t="s">
         <v>599</v>
       </c>
@@ -6214,7 +6360,9 @@
       <c r="C131" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D131" s="6"/>
+      <c r="D131" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E131" s="4" t="s">
         <v>600</v>
       </c>
@@ -6241,7 +6389,9 @@
       <c r="C132" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D132" s="6"/>
+      <c r="D132" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E132" s="4" t="s">
         <v>601</v>
       </c>
@@ -6268,7 +6418,9 @@
       <c r="C133" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D133" s="6"/>
+      <c r="D133" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E133" s="4" t="s">
         <v>602</v>
       </c>
@@ -6295,7 +6447,9 @@
       <c r="C134" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D134" s="6"/>
+      <c r="D134" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E134" s="4" t="s">
         <v>603</v>
       </c>
@@ -6322,7 +6476,9 @@
       <c r="C135" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D135" s="6"/>
+      <c r="D135" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E135" s="4" t="s">
         <v>604</v>
       </c>
@@ -6349,7 +6505,9 @@
       <c r="C136" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D136" s="6"/>
+      <c r="D136" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E136" s="4" t="s">
         <v>605</v>
       </c>
@@ -6376,7 +6534,9 @@
       <c r="C137" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D137" s="6"/>
+      <c r="D137" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E137" s="4" t="s">
         <v>606</v>
       </c>
@@ -6403,7 +6563,9 @@
       <c r="C138" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D138" s="6"/>
+      <c r="D138" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E138" s="4" t="s">
         <v>607</v>
       </c>
@@ -6430,7 +6592,9 @@
       <c r="C139" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D139" s="6"/>
+      <c r="D139" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E139" s="4" t="s">
         <v>608</v>
       </c>
@@ -6457,7 +6621,9 @@
       <c r="C140" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D140" s="6"/>
+      <c r="D140" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E140" s="4" t="s">
         <v>609</v>
       </c>
@@ -6484,7 +6650,9 @@
       <c r="C141" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D141" s="6"/>
+      <c r="D141" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E141" s="4" t="s">
         <v>610</v>
       </c>
@@ -6511,7 +6679,9 @@
       <c r="C142" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D142" s="6"/>
+      <c r="D142" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E142" s="4" t="s">
         <v>611</v>
       </c>
@@ -6538,7 +6708,9 @@
       <c r="C143" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D143" s="6"/>
+      <c r="D143" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E143" s="4" t="s">
         <v>612</v>
       </c>
@@ -6565,7 +6737,9 @@
       <c r="C144" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D144" s="6"/>
+      <c r="D144" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E144" s="4" t="s">
         <v>613</v>
       </c>
@@ -6592,7 +6766,9 @@
       <c r="C145" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D145" s="6"/>
+      <c r="D145" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E145" s="4" t="s">
         <v>614</v>
       </c>
@@ -6619,7 +6795,9 @@
       <c r="C146" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D146" s="6"/>
+      <c r="D146" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E146" s="4" t="s">
         <v>615</v>
       </c>
@@ -6646,7 +6824,9 @@
       <c r="C147" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D147" s="6"/>
+      <c r="D147" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E147" s="4" t="s">
         <v>616</v>
       </c>
@@ -6673,7 +6853,9 @@
       <c r="C148" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D148" s="6"/>
+      <c r="D148" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E148" s="4" t="s">
         <v>617</v>
       </c>
@@ -6700,7 +6882,9 @@
       <c r="C149" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D149" s="6"/>
+      <c r="D149" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E149" s="4" t="s">
         <v>618</v>
       </c>
@@ -6727,7 +6911,9 @@
       <c r="C150" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D150" s="6"/>
+      <c r="D150" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E150" s="4" t="s">
         <v>619</v>
       </c>
@@ -6755,7 +6941,9 @@
       <c r="C151" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D151" s="6"/>
+      <c r="D151" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E151" s="4" t="s">
         <v>620</v>
       </c>
@@ -6782,7 +6970,9 @@
       <c r="C152" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D152" s="6"/>
+      <c r="D152" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E152" s="4" t="s">
         <v>621</v>
       </c>
@@ -6809,7 +6999,9 @@
       <c r="C153" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D153" s="6"/>
+      <c r="D153" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E153" s="4" t="s">
         <v>622</v>
       </c>
@@ -6836,7 +7028,9 @@
       <c r="C154" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D154" s="6"/>
+      <c r="D154" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E154" s="4" t="s">
         <v>623</v>
       </c>
@@ -6863,7 +7057,9 @@
       <c r="C155" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D155" s="6"/>
+      <c r="D155" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E155" s="4" t="s">
         <v>624</v>
       </c>
@@ -6890,7 +7086,9 @@
       <c r="C156" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D156" s="8"/>
+      <c r="D156" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E156" s="4" t="s">
         <v>625</v>
       </c>
@@ -7324,7 +7522,9 @@
       <c r="C171" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D171" s="1"/>
+      <c r="D171" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E171" s="4" t="s">
         <v>639</v>
       </c>
@@ -7351,7 +7551,9 @@
       <c r="C172" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D172" s="1"/>
+      <c r="D172" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E172" s="4" t="s">
         <v>640</v>
       </c>
@@ -7379,7 +7581,9 @@
       <c r="C173" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D173" s="1"/>
+      <c r="D173" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E173" s="4" t="s">
         <v>641</v>
       </c>
@@ -7406,7 +7610,9 @@
       <c r="C174" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D174" s="1"/>
+      <c r="D174" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E174" s="4" t="s">
         <v>642</v>
       </c>
@@ -7434,7 +7640,9 @@
       <c r="C175" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D175" s="1"/>
+      <c r="D175" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E175" s="4" t="s">
         <v>643</v>
       </c>
@@ -7461,7 +7669,9 @@
       <c r="C176" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D176" s="1"/>
+      <c r="D176" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E176" s="4" t="s">
         <v>644</v>
       </c>
@@ -7488,7 +7698,9 @@
       <c r="C177" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D177" s="1"/>
+      <c r="D177" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E177" s="4" t="s">
         <v>645</v>
       </c>
@@ -7515,7 +7727,9 @@
       <c r="C178" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D178" s="1"/>
+      <c r="D178" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E178" s="4" t="s">
         <v>646</v>
       </c>
@@ -7542,7 +7756,9 @@
       <c r="C179" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D179" s="1"/>
+      <c r="D179" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E179" s="4" t="s">
         <v>647</v>
       </c>
@@ -7569,7 +7785,9 @@
       <c r="C180" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D180" s="1"/>
+      <c r="D180" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E180" s="4" t="s">
         <v>648</v>
       </c>
@@ -7596,7 +7814,9 @@
       <c r="C181" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D181" s="1"/>
+      <c r="D181" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E181" s="4" t="s">
         <v>649</v>
       </c>
@@ -7623,7 +7843,9 @@
       <c r="C182" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D182" s="1"/>
+      <c r="D182" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="E182" s="4" t="s">
         <v>650</v>
       </c>
@@ -7650,7 +7872,9 @@
       <c r="C183" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D183" s="1"/>
+      <c r="D183" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E183" s="4" t="s">
         <v>651</v>
       </c>
@@ -7677,7 +7901,9 @@
       <c r="C184" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D184" s="1"/>
+      <c r="D184" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="E184" s="4" t="s">
         <v>652</v>
       </c>

</xml_diff>